<commit_message>
Added fix for duration histogram labels
</commit_message>
<xml_diff>
--- a/public/data/analysis.xlsx
+++ b/public/data/analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/sbu/cse564/lab1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/sbu/cse564/lab1/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E9A3EC-6D17-0C4F-9EEA-A356C6D95EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A149BD45-D06F-9C4D-8207-6AE74B8CEC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="820" windowWidth="27940" windowHeight="17440" xr2:uid="{02C18367-2CEF-CE46-BAE6-BA525A5A4D19}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$Q$501</definedName>
     <definedName name="out" localSheetId="0">Sheet2!$C$1:$D$501</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -4967,8 +4967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDD872F-9458-A247-BC92-20CCBBE4E7A8}">
   <dimension ref="A1:Q501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31539,7 +31539,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{8FDD872F-9458-A247-BC92-20CCBBE4E7A8}">
+  <autoFilter ref="A1:Q501" xr:uid="{8FDD872F-9458-A247-BC92-20CCBBE4E7A8}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q501">
       <sortCondition ref="J1:J501"/>
     </sortState>

</xml_diff>